<commit_message>
- ADD: Added markers field to configuration. - CHG: Updated GridScore Germinate export to latest version of templates.
</commit_message>
<xml_diff>
--- a/src/main/resources/trials-data.xlsx
+++ b/src/main/resources/trials-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\trials-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F8B1C7-5368-4163-A191-BA082635DF6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C41157-65CA-43E3-A647-B77A09BF3879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -345,6 +349,57 @@
   <si>
     <t>B</t>
   </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Investigation Title</t>
+  </si>
+  <si>
+    <t>Human-readable string summarising the investigation.</t>
+  </si>
+  <si>
+    <t>Investigation Description</t>
+  </si>
+  <si>
+    <t>Human-readable text describing the investigation in more detail.</t>
+  </si>
+  <si>
+    <t>Investigation unique ID</t>
+  </si>
+  <si>
+    <t>Identifier comprising the unique name of the institution/database hosting the submission of the investigation data, and the accession number of the investigation in that institution.</t>
+  </si>
+  <si>
+    <t>Associated data file link</t>
+  </si>
+  <si>
+    <t>Link to the data file (or digital object) in a public database or in a persistent institutional repository; or identifier of the data file when submitted together with the MIAPPE submission.</t>
+  </si>
+  <si>
+    <t>Associated data file description</t>
+  </si>
+  <si>
+    <t>Description of the format of the data file. May be a standard file format name, or a description of organization of the data in a tabular file.</t>
+  </si>
+  <si>
+    <t>Associated data file version</t>
+  </si>
+  <si>
+    <t>The version of the dataset (the actual data).</t>
+  </si>
+  <si>
+    <t>Contributor role</t>
+  </si>
+  <si>
+    <t>Contributor ID</t>
+  </si>
+  <si>
+    <t>Type of contribution of the person to the investigation (e.g. data submitter; author; corresponding author)</t>
+  </si>
+  <si>
+    <t>An identifier for the data submitter. If that submitter is an individual, ORCID identifiers are recommended.</t>
+  </si>
 </sst>
 </file>
 
@@ -353,7 +408,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyymmdd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,6 +475,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -462,7 +523,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -528,6 +589,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -535,13 +605,24 @@
     <cellStyle name="Normal 4" xfId="1" xr:uid="{AC6FD0CA-C916-4E1F-8927-7A9CF5AB4487}"/>
     <cellStyle name="Warning Text" xfId="3" builtinId="11"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="27">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -558,15 +639,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -580,6 +652,44 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -688,6 +798,13 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -712,8 +829,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="21"/>
-      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -728,25 +845,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:C12" xr:uid="{DCA4608A-E2D9-45F1-81E3-F49396F38526}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:C18" xr:uid="{DCA4608A-E2D9-45F1-81E3-F49396F38526}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:H12" totalsRowShown="0">
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:L12" totalsRowShown="0">
+  <autoFilter ref="A1:L12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Line/Phenotype"/>
     <tableColumn id="2" xr3:uid="{CB956365-108C-47D3-B28E-EBDFD6E16995}" name="Rep"/>
+    <tableColumn id="9" xr3:uid="{8C52E70E-74F2-424A-8F55-980BEB83541C}" name="Block"/>
     <tableColumn id="7" xr3:uid="{88B30358-C3FE-4E11-B08D-42FB21CD6479}" name="Treatment"/>
     <tableColumn id="8" xr3:uid="{13CC7C54-6C19-41EF-BA0D-75E84678E993}" name="Location"/>
+    <tableColumn id="10" xr3:uid="{4DB6F789-093F-4C73-B982-C2E54070E165}" name="Latitude" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{7DF6B222-3988-4F46-991B-F6C2F213B41D}" name="Longitude" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{55ED41BA-9315-4A55-B989-C3614B9C3340}" name="Elevation" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Ear length"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Ear number per plant"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Ear width"/>
@@ -757,16 +878,20 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table44" displayName="Table44" ref="A1:G12" totalsRowShown="0">
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table44" displayName="Table44" ref="A1:K12" totalsRowShown="0">
+  <autoFilter ref="A1:K12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Line/Phenotype"/>
     <tableColumn id="7" xr3:uid="{F56FA6B6-097B-4A91-BE3C-84316559494C}" name="Rep"/>
+    <tableColumn id="8" xr3:uid="{B1199833-CBFA-4386-8BC3-8225F4549F7B}" name="Block"/>
     <tableColumn id="2" xr3:uid="{372B6450-E223-4B62-BE37-A66868D227D6}" name="Treatment"/>
     <tableColumn id="5" xr3:uid="{5F0A8F5E-5F8D-498B-AA15-759C67F77D36}" name="Location"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Ear length" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Ear number per plant" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Ear width" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{907497DD-05CD-436D-8F9D-C9733135B6D1}" name="Latitude"/>
+    <tableColumn id="10" xr3:uid="{F68843F4-17C8-471E-8FEA-8A1CF9BD7F9F}" name="Longitude"/>
+    <tableColumn id="9" xr3:uid="{97B62C49-64CB-4474-93B9-41298499FF28}" name="Elevation"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Ear length" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Ear number per plant" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Ear width" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -800,16 +925,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:G2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:G2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
-  <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
+  <tableColumns count="9">
+    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{B35B0A33-6132-493B-9131-6BA92C731A13}" name="Contributor role" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{901F3798-43D3-40F0-8C23-0793303EE87C}" name="Contributor ID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -835,26 +962,34 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22E566EA-CF41-4BD4-A877-BF1A04CBE27C}" name="Table47" displayName="Table47" ref="A1:D2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22E566EA-CF41-4BD4-A877-BF1A04CBE27C}" name="Table47" displayName="Table47" ref="A1:H2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{CCD80E05-5388-423E-BBDC-2354AB7B8FC3}" name="Line/Phenotype"/>
     <tableColumn id="2" xr3:uid="{466AEB02-1AD0-430A-B6D8-FF71A9F751B4}" name="Rep"/>
+    <tableColumn id="8" xr3:uid="{B32A4B56-1C05-4F7B-B51B-4FA3967354E2}" name="Block"/>
     <tableColumn id="7" xr3:uid="{40C0F606-B99C-4595-806C-A7295CC796D9}" name="Treatment"/>
     <tableColumn id="3" xr3:uid="{8EE9A1A1-AEF3-490F-B2E4-D6A460210A54}" name="Location"/>
+    <tableColumn id="4" xr3:uid="{69C9CE63-BD11-4E4B-957D-A99D3AA2F63C}" name="Latitude"/>
+    <tableColumn id="5" xr3:uid="{67FFEBA5-AD32-417A-987A-2C040AA24764}" name="Longitude"/>
+    <tableColumn id="6" xr3:uid="{D986DFA6-2CBB-40DF-84E8-21CC5C183E1E}" name="Elevation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E9D794-B34F-44CE-84F6-AA0D14CDB5C6}" name="Table4411" displayName="Table4411" ref="A1:D2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{7A5E0959-3CB3-48DB-A1FB-2A58B80F3191}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E9D794-B34F-44CE-84F6-AA0D14CDB5C6}" name="Table4411" displayName="Table4411" ref="A1:H2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{7A5E0959-3CB3-48DB-A1FB-2A58B80F3191}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{4C72BB57-561C-4C97-9A88-82A2D428A82A}" name="Line/Phenotype"/>
     <tableColumn id="7" xr3:uid="{D9EE74B9-83DA-4C06-B461-5A4F7DC2FD15}" name="Rep"/>
+    <tableColumn id="4" xr3:uid="{57727AAB-E4BF-42AD-962C-0DBC24A599A0}" name="Block"/>
     <tableColumn id="2" xr3:uid="{233E7CDA-E23F-4F59-95B7-C14E55E139E2}" name="Treatment"/>
     <tableColumn id="3" xr3:uid="{9976F5CF-934C-4F0C-8E8C-314FBD437428}" name="Location"/>
+    <tableColumn id="5" xr3:uid="{2F3B018F-D870-41DE-A4AF-30757F61E6A4}" name="Latitude"/>
+    <tableColumn id="6" xr3:uid="{8AFBB6FA-5BB0-4119-9890-AECAE760BE7C}" name="Longitude"/>
+    <tableColumn id="8" xr3:uid="{5C5F4AEC-9A07-4522-92E5-02F8A657C494}" name="Elevation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1157,9 +1292,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1285,51 +1420,105 @@
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="31"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A14" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="31"/>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="31"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="31"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="31"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B21" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="13"/>
-    </row>
-    <row r="17" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="13"/>
+    </row>
+    <row r="23" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B25" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B27" s="19" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="24" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1346,25 +1535,28 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D12"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1372,304 +1564,449 @@
         <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
+        <v>56.46152</v>
+      </c>
+      <c r="G2" s="4">
+        <v>-3.1109200000000001</v>
+      </c>
+      <c r="H2" s="4">
+        <v>38.9</v>
+      </c>
+      <c r="I2" s="4">
         <v>15.698600000000001</v>
       </c>
-      <c r="F2" s="4">
+      <c r="J2" s="4">
         <v>7</v>
       </c>
-      <c r="G2" s="4">
+      <c r="K2" s="4">
         <v>20.435199999999998</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
+        <v>56.470471000000003</v>
+      </c>
+      <c r="G3" s="4">
+        <v>-3.1227999999999998</v>
+      </c>
+      <c r="H3" s="4">
+        <v>26.4</v>
+      </c>
+      <c r="I3" s="4">
         <v>17.075500000000002</v>
       </c>
-      <c r="F3" s="4">
+      <c r="J3" s="4">
         <v>8</v>
       </c>
-      <c r="G3" s="4">
+      <c r="K3" s="4">
         <v>24.342500000000001</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
+        <v>56.465794000000002</v>
+      </c>
+      <c r="G4" s="4">
+        <v>-3.12696</v>
+      </c>
+      <c r="H4" s="4">
+        <v>98.1</v>
+      </c>
+      <c r="I4" s="4">
         <v>5.6565000000000003</v>
       </c>
-      <c r="F4" s="4">
+      <c r="J4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="K4" s="4">
         <v>10.432399999999999</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
+        <v>56.468415</v>
+      </c>
+      <c r="G5" s="4">
+        <v>-3.1256499999999998</v>
+      </c>
+      <c r="H5" s="4">
+        <v>76.5</v>
+      </c>
+      <c r="I5" s="4">
         <v>6.4452999999999996</v>
       </c>
-      <c r="F5" s="4">
+      <c r="J5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="K5" s="4">
         <v>9.4054000000000002</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
+        <v>56.470269999999999</v>
+      </c>
+      <c r="G6" s="4">
+        <v>-3.1406999999999998</v>
+      </c>
+      <c r="H6" s="4">
+        <v>76.2</v>
+      </c>
+      <c r="I6" s="4">
         <v>16.232500000000002</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4">
         <v>21.435600000000001</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
+        <v>56.471969000000001</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-3.11985</v>
+      </c>
+      <c r="H7" s="4">
+        <v>62.4</v>
+      </c>
+      <c r="I7" s="4">
         <v>17.552600000000002</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4">
         <v>22.467400000000001</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="4">
+        <v>56.468760000000003</v>
+      </c>
+      <c r="G8" s="4">
+        <v>-3.1153</v>
+      </c>
+      <c r="H8" s="4">
+        <v>56.4</v>
+      </c>
+      <c r="I8" s="4">
         <v>4.5321999999999996</v>
       </c>
-      <c r="F8" s="4">
+      <c r="J8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="4">
+      <c r="K8" s="4">
         <v>16.546600000000002</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
+        <v>56.467841999999997</v>
+      </c>
+      <c r="G9" s="4">
+        <v>-3.1088</v>
+      </c>
+      <c r="H9" s="4">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="I9" s="4">
         <v>6.3562000000000003</v>
       </c>
-      <c r="F9" s="4">
+      <c r="J9" s="4">
         <v>3</v>
       </c>
-      <c r="G9" s="4">
+      <c r="K9" s="4">
         <v>15.545299999999999</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="4">
+        <v>56.469270999999999</v>
+      </c>
+      <c r="G10" s="4">
+        <v>-3.14317</v>
+      </c>
+      <c r="H10" s="4">
+        <v>85.6</v>
+      </c>
+      <c r="I10">
         <v>14.5463</v>
       </c>
-      <c r="F10">
+      <c r="J10">
         <v>6</v>
       </c>
-      <c r="G10">
+      <c r="K10">
         <v>24.545300000000001</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="L10" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E11">
+      <c r="F11" s="4">
+        <v>56.472653000000001</v>
+      </c>
+      <c r="G11" s="4">
+        <v>-3.1432699999999998</v>
+      </c>
+      <c r="H11" s="4">
+        <v>23.6</v>
+      </c>
+      <c r="I11">
         <v>20.435600000000001</v>
       </c>
-      <c r="F11">
+      <c r="J11">
         <v>8</v>
       </c>
-      <c r="G11">
+      <c r="K11">
         <v>25.5366</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="4">
+        <v>56.461801000000001</v>
+      </c>
+      <c r="G12" s="4">
+        <v>-3.1385399999999999</v>
+      </c>
+      <c r="H12" s="4">
+        <v>85.9</v>
+      </c>
+      <c r="J12">
         <v>1</v>
       </c>
-      <c r="G12">
+      <c r="K12">
         <v>9.4344999999999999</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1682,25 +2019,26 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1708,303 +2046,447 @@
         <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="4">
+        <v>56.46152</v>
+      </c>
+      <c r="G2" s="4">
+        <v>-3.1109200000000001</v>
+      </c>
+      <c r="H2" s="4">
+        <v>38.9</v>
+      </c>
+      <c r="I2" s="5">
         <v>42371</v>
       </c>
-      <c r="F2" s="5">
+      <c r="J2" s="5">
         <v>42373</v>
       </c>
-      <c r="G2" s="5">
+      <c r="K2" s="5">
         <v>42373</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="4">
+        <v>56.470471000000003</v>
+      </c>
+      <c r="G3" s="4">
+        <v>-3.1227999999999998</v>
+      </c>
+      <c r="H3" s="4">
+        <v>26.4</v>
+      </c>
+      <c r="I3" s="5">
         <v>42370</v>
       </c>
-      <c r="F3" s="5">
+      <c r="J3" s="5">
         <v>42375</v>
       </c>
-      <c r="G3" s="5">
+      <c r="K3" s="5">
         <v>42370</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="4">
+        <v>56.465794000000002</v>
+      </c>
+      <c r="G4" s="4">
+        <v>-3.12696</v>
+      </c>
+      <c r="H4" s="4">
+        <v>98.1</v>
+      </c>
+      <c r="I4" s="5">
         <v>42377</v>
       </c>
-      <c r="F4" s="5">
+      <c r="J4" s="5">
         <v>42372</v>
       </c>
-      <c r="G4" s="5">
+      <c r="K4" s="5">
         <v>42377</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="4">
+        <v>56.468415</v>
+      </c>
+      <c r="G5" s="4">
+        <v>-3.1256499999999998</v>
+      </c>
+      <c r="H5" s="4">
+        <v>76.5</v>
+      </c>
+      <c r="I5" s="5">
         <v>42378</v>
       </c>
-      <c r="F5" s="5">
+      <c r="J5" s="5">
         <v>42377</v>
       </c>
-      <c r="G5" s="5">
+      <c r="K5" s="5">
         <v>42374</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="4">
+        <v>56.470269999999999</v>
+      </c>
+      <c r="G6" s="4">
+        <v>-3.1406999999999998</v>
+      </c>
+      <c r="H6" s="4">
+        <v>76.2</v>
+      </c>
+      <c r="I6" s="5">
         <v>42376</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5">
         <v>42373</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="4">
+        <v>56.471969000000001</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-3.11985</v>
+      </c>
+      <c r="H7" s="4">
+        <v>62.4</v>
+      </c>
+      <c r="I7" s="5">
         <v>42374</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5">
         <v>42375</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="4">
+        <v>56.468760000000003</v>
+      </c>
+      <c r="G8" s="4">
+        <v>-3.1153</v>
+      </c>
+      <c r="H8" s="4">
+        <v>56.4</v>
+      </c>
+      <c r="I8" s="5">
         <v>42371</v>
       </c>
-      <c r="F8" s="5">
+      <c r="J8" s="5">
         <v>42374</v>
       </c>
-      <c r="G8" s="5">
+      <c r="K8" s="5">
         <v>42376</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="4">
+        <v>56.467841999999997</v>
+      </c>
+      <c r="G9" s="4">
+        <v>-3.1088</v>
+      </c>
+      <c r="H9" s="4">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="I9" s="5">
         <v>42379</v>
       </c>
-      <c r="F9" s="5">
+      <c r="J9" s="5">
         <v>42376</v>
       </c>
-      <c r="G9" s="5">
+      <c r="K9" s="5">
         <v>42373</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="4">
+        <v>56.469270999999999</v>
+      </c>
+      <c r="G10" s="4">
+        <v>-3.14317</v>
+      </c>
+      <c r="H10" s="4">
+        <v>85.6</v>
+      </c>
+      <c r="I10" s="5">
         <v>42373</v>
       </c>
-      <c r="F10" s="5">
+      <c r="J10" s="5">
         <v>42374</v>
       </c>
-      <c r="G10" s="5">
+      <c r="K10" s="5">
         <v>42376</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="4">
+        <v>56.472653000000001</v>
+      </c>
+      <c r="G11" s="4">
+        <v>-3.1432699999999998</v>
+      </c>
+      <c r="H11" s="4">
+        <v>23.6</v>
+      </c>
+      <c r="I11" s="5">
         <v>42379</v>
       </c>
-      <c r="F11" s="5">
+      <c r="J11" s="5">
         <v>42376</v>
       </c>
-      <c r="G11" s="5">
+      <c r="K11" s="5">
         <v>42374</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
+        <v>56.461801000000001</v>
+      </c>
+      <c r="G12" s="4">
+        <v>-3.1385399999999999</v>
+      </c>
+      <c r="H12" s="4">
+        <v>85.9</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5">
         <v>42370</v>
       </c>
-      <c r="G12" s="5">
+      <c r="K12" s="5">
         <v>42372</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F20" s="5"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:D1" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:H1" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -2081,7 +2563,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,67 +2610,79 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2115B6D0-8EC1-4029-B8F6-04E7D9736B3A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" style="23" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="25" style="23" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="23" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="23"/>
+    <col min="2" max="4" width="40.85546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="25" style="23" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="H2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="I2" s="21" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2303,7 +2797,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2 D2">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2330,19 +2824,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="9" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>7</v>
       </c>
@@ -2350,70 +2847,82 @@
         <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2430,20 +2939,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2451,20 +2961,32 @@
         <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
   </sheetData>
   <dataValidations xWindow="96" yWindow="450" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:C1" xr:uid="{13E30841-E8AE-4AEA-9BB5-750247107F69}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:D1" xr:uid="{13E30841-E8AE-4AEA-9BB5-750247107F69}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2480,7 +3002,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- ADD: Added shapefile export. - CHG: Updated Germinate trials data template to latest version including row/column numbers. - CHG: Updated config joiner to support rep numbers. -
</commit_message>
<xml_diff>
--- a/src/main/resources/trials-data.xlsx
+++ b/src/main/resources/trials-data.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\trials-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C41157-65CA-43E3-A647-B77A09BF3879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CD3032-92FE-4E67-BDD9-F1701119FD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
-    <sheet name="ATTRIBUTES" sheetId="11" r:id="rId2"/>
-    <sheet name="LOCATION" sheetId="10" r:id="rId3"/>
-    <sheet name="COLLABORATORS" sheetId="9" r:id="rId4"/>
-    <sheet name="PHENOTYPES" sheetId="2" r:id="rId5"/>
-    <sheet name="DATA" sheetId="6" r:id="rId6"/>
-    <sheet name="RECORDING_DATES" sheetId="7" r:id="rId7"/>
+    <sheet name="PHENOTYPES" sheetId="2" r:id="rId2"/>
+    <sheet name="DATA" sheetId="6" r:id="rId3"/>
+    <sheet name="RECORDING_DATES" sheetId="7" r:id="rId4"/>
+    <sheet name="ATTRIBUTES" sheetId="11" r:id="rId5"/>
+    <sheet name="COLLABORATORS" sheetId="9" r:id="rId6"/>
+    <sheet name="LOCATION" sheetId="10" r:id="rId7"/>
     <sheet name="LOCATION_EXAMPLE" sheetId="12" r:id="rId8"/>
     <sheet name="PHENOTYPES_EXAMPLE" sheetId="5" r:id="rId9"/>
     <sheet name="DATA_EXAMPLE" sheetId="4" r:id="rId10"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Additional Information</t>
-  </si>
-  <si>
-    <t>Please include any additional information that details how this experiment was carried out in a text or Word document and send along with this template. If there are any images please send these as individual JPG files.</t>
   </si>
   <si>
     <t>Help and Assistance</t>
@@ -399,6 +396,15 @@
   </si>
   <si>
     <t>An identifier for the data submitter. If that submitter is an individual, ORCID identifiers are recommended.</t>
+  </si>
+  <si>
+    <t>Please include any additional information that details how this experiment was carried out in a text or Word document and send along with this template. If there are any images please send these as individual JPG files. Mandatory fields are highlighted in yellow.</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Column</t>
   </si>
 </sst>
 </file>
@@ -556,9 +562,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -598,6 +601,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -606,6 +612,27 @@
     <cellStyle name="Warning Text" xfId="3" builtinId="11"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyymmdd"/>
     </dxf>
@@ -623,20 +650,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -798,13 +811,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -845,29 +851,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:C18" xr:uid="{DCA4608A-E2D9-45F1-81E3-F49396F38526}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:L12" totalsRowShown="0">
-  <autoFilter ref="A1:L12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:N12" totalsRowShown="0">
+  <autoFilter ref="A1:N12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Line/Phenotype"/>
     <tableColumn id="2" xr3:uid="{CB956365-108C-47D3-B28E-EBDFD6E16995}" name="Rep"/>
     <tableColumn id="9" xr3:uid="{8C52E70E-74F2-424A-8F55-980BEB83541C}" name="Block"/>
+    <tableColumn id="13" xr3:uid="{20544D5A-2E37-40C0-8903-7DFE8E1801E4}" name="Row"/>
+    <tableColumn id="14" xr3:uid="{CE255CEA-3127-418C-9432-3F63F51FD781}" name="Column"/>
     <tableColumn id="7" xr3:uid="{88B30358-C3FE-4E11-B08D-42FB21CD6479}" name="Treatment"/>
     <tableColumn id="8" xr3:uid="{13CC7C54-6C19-41EF-BA0D-75E84678E993}" name="Location"/>
-    <tableColumn id="10" xr3:uid="{4DB6F789-093F-4C73-B982-C2E54070E165}" name="Latitude" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{7DF6B222-3988-4F46-991B-F6C2F213B41D}" name="Longitude" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{55ED41BA-9315-4A55-B989-C3614B9C3340}" name="Elevation" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{4DB6F789-093F-4C73-B982-C2E54070E165}" name="Latitude" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{7DF6B222-3988-4F46-991B-F6C2F213B41D}" name="Longitude" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{55ED41BA-9315-4A55-B989-C3614B9C3340}" name="Elevation" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Ear length"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Ear number per plant"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Ear width"/>
@@ -889,60 +897,15 @@
     <tableColumn id="11" xr3:uid="{907497DD-05CD-436D-8F9D-C9733135B6D1}" name="Latitude"/>
     <tableColumn id="10" xr3:uid="{F68843F4-17C8-471E-8FEA-8A1CF9BD7F9F}" name="Longitude"/>
     <tableColumn id="9" xr3:uid="{97B62C49-64CB-4474-93B9-41298499FF28}" name="Elevation"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Ear length" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Ear number per plant" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Ear width" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Ear length" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Ear number per plant" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Ear width" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61617974-7B97-4C3B-BA5A-15C9DF6B5915}" name="Table1" displayName="Table1" ref="A1:C2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:C2" xr:uid="{AFAF2A04-D11A-4761-ABA6-DA7D533456A3}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6687827E-20FF-44CC-820C-7FCA95E05637}" name="Attribute"/>
-    <tableColumn id="3" xr3:uid="{E9386995-F6BE-45FD-B47F-6F50A0356B8E}" name="Type"/>
-    <tableColumn id="2" xr3:uid="{9A9860D2-E2EF-4AF1-AF01-F935BF554D92}" name="Value"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{54BDA44A-CD87-4E45-AED3-C04513F7E914}" name="Table9" displayName="Table9" ref="A1:F2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{F62B6A96-E1F2-40B5-8B32-4E4F94F6494A}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A8F49BB-5B5C-4DA6-BCFF-0458FF526B9E}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{5863ACB9-3750-47DF-B55F-40C0B119E7E4}" name="Short name"/>
-    <tableColumn id="3" xr3:uid="{C3E73087-AAA0-4C32-A529-1FB205F5DCCE}" name="Country"/>
-    <tableColumn id="4" xr3:uid="{ECF010CE-69C0-49B6-84B9-F22057CDAFB0}" name="Elevation"/>
-    <tableColumn id="5" xr3:uid="{A7D62594-421F-420D-AF72-E3320E9B4E38}" name="Latitude"/>
-    <tableColumn id="6" xr3:uid="{1F86E5D8-33FD-45F7-87AD-13D2B6EDCA41}" name="Longitude"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
-  <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{B35B0A33-6132-493B-9131-6BA92C731A13}" name="Contributor role" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{901F3798-43D3-40F0-8C23-0793303EE87C}" name="Contributor ID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDF6150C-EB7C-4511-B47B-2F8122570053}" name="Table136" displayName="Table136" ref="A1:J2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:J2" xr:uid="{4E670C69-5459-4D42-BBD4-1C0FE57A115B}"/>
   <tableColumns count="10">
@@ -961,13 +924,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22E566EA-CF41-4BD4-A877-BF1A04CBE27C}" name="Table47" displayName="Table47" ref="A1:H2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
-  <tableColumns count="8">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22E566EA-CF41-4BD4-A877-BF1A04CBE27C}" name="Table47" displayName="Table47" ref="A1:J2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{CCD80E05-5388-423E-BBDC-2354AB7B8FC3}" name="Line/Phenotype"/>
     <tableColumn id="2" xr3:uid="{466AEB02-1AD0-430A-B6D8-FF71A9F751B4}" name="Rep"/>
     <tableColumn id="8" xr3:uid="{B32A4B56-1C05-4F7B-B51B-4FA3967354E2}" name="Block"/>
+    <tableColumn id="9" xr3:uid="{2ED92832-AD7D-4A22-8917-F561E101C555}" name="Row"/>
+    <tableColumn id="10" xr3:uid="{61C248C8-9EF3-432C-BE20-51527617EB5B}" name="Column"/>
     <tableColumn id="7" xr3:uid="{40C0F606-B99C-4595-806C-A7295CC796D9}" name="Treatment"/>
     <tableColumn id="3" xr3:uid="{8EE9A1A1-AEF3-490F-B2E4-D6A460210A54}" name="Location"/>
     <tableColumn id="4" xr3:uid="{69C9CE63-BD11-4E4B-957D-A99D3AA2F63C}" name="Latitude"/>
@@ -978,18 +943,65 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E9D794-B34F-44CE-84F6-AA0D14CDB5C6}" name="Table4411" displayName="Table4411" ref="A1:H2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{7A5E0959-3CB3-48DB-A1FB-2A58B80F3191}"/>
-  <tableColumns count="8">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E9D794-B34F-44CE-84F6-AA0D14CDB5C6}" name="Table4411" displayName="Table4411" ref="A1:J2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{7A5E0959-3CB3-48DB-A1FB-2A58B80F3191}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4C72BB57-561C-4C97-9A88-82A2D428A82A}" name="Line/Phenotype"/>
     <tableColumn id="7" xr3:uid="{D9EE74B9-83DA-4C06-B461-5A4F7DC2FD15}" name="Rep"/>
     <tableColumn id="4" xr3:uid="{57727AAB-E4BF-42AD-962C-0DBC24A599A0}" name="Block"/>
+    <tableColumn id="9" xr3:uid="{01A0EDA9-30E9-4526-A528-8A71ADD7B449}" name="Row"/>
+    <tableColumn id="10" xr3:uid="{C40DC8EF-6D3A-43F0-B3FC-4A7CF45DCFE4}" name="Column"/>
     <tableColumn id="2" xr3:uid="{233E7CDA-E23F-4F59-95B7-C14E55E139E2}" name="Treatment"/>
     <tableColumn id="3" xr3:uid="{9976F5CF-934C-4F0C-8E8C-314FBD437428}" name="Location"/>
     <tableColumn id="5" xr3:uid="{2F3B018F-D870-41DE-A4AF-30757F61E6A4}" name="Latitude"/>
     <tableColumn id="6" xr3:uid="{8AFBB6FA-5BB0-4119-9890-AECAE760BE7C}" name="Longitude"/>
     <tableColumn id="8" xr3:uid="{5C5F4AEC-9A07-4522-92E5-02F8A657C494}" name="Elevation"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61617974-7B97-4C3B-BA5A-15C9DF6B5915}" name="Table1" displayName="Table1" ref="A1:C2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:C2" xr:uid="{AFAF2A04-D11A-4761-ABA6-DA7D533456A3}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6687827E-20FF-44CC-820C-7FCA95E05637}" name="Attribute"/>
+    <tableColumn id="3" xr3:uid="{E9386995-F6BE-45FD-B47F-6F50A0356B8E}" name="Type"/>
+    <tableColumn id="2" xr3:uid="{9A9860D2-E2EF-4AF1-AF01-F935BF554D92}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
+  <tableColumns count="9">
+    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{B35B0A33-6132-493B-9131-6BA92C731A13}" name="Contributor role" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{901F3798-43D3-40F0-8C23-0793303EE87C}" name="Contributor ID" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{54BDA44A-CD87-4E45-AED3-C04513F7E914}" name="Table9" displayName="Table9" ref="A1:F2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{F62B6A96-E1F2-40B5-8B32-4E4F94F6494A}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8A8F49BB-5B5C-4DA6-BCFF-0458FF526B9E}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{5863ACB9-3750-47DF-B55F-40C0B119E7E4}" name="Short name"/>
+    <tableColumn id="3" xr3:uid="{C3E73087-AAA0-4C32-A529-1FB205F5DCCE}" name="Country"/>
+    <tableColumn id="4" xr3:uid="{ECF010CE-69C0-49B6-84B9-F22057CDAFB0}" name="Elevation"/>
+    <tableColumn id="5" xr3:uid="{A7D62594-421F-420D-AF72-E3320E9B4E38}" name="Latitude"/>
+    <tableColumn id="6" xr3:uid="{1F86E5D8-33FD-45F7-87AD-13D2B6EDCA41}" name="Longitude"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1294,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,102 +1323,102 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>37</v>
-      </c>
       <c r="B2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="20"/>
+        <v>48</v>
+      </c>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="C11" s="9"/>
     </row>
@@ -1415,63 +1427,63 @@
         <v>4</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="C13" s="30"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="31"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="B14" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="C14" s="30"/>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="31"/>
-    </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="B15" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="C15" s="30"/>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="31"/>
-    </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="B16" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="C16" s="30"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="31"/>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="B17" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="C17" s="30"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="31"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="B18" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="31"/>
+      <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
@@ -1486,7 +1498,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1500,25 +1512,25 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>34</v>
+      <c r="B27" s="18" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="containsBlanks" dxfId="24" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1535,68 +1547,74 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="6.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1604,37 +1622,43 @@
       <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="4">
         <v>56.46152</v>
       </c>
-      <c r="G2" s="4">
+      <c r="I2" s="4">
         <v>-3.1109200000000001</v>
       </c>
-      <c r="H2" s="4">
+      <c r="J2" s="4">
         <v>38.9</v>
       </c>
-      <c r="I2" s="4">
+      <c r="K2" s="4">
         <v>15.698600000000001</v>
       </c>
-      <c r="J2" s="4">
+      <c r="L2" s="4">
         <v>7</v>
       </c>
-      <c r="K2" s="4">
+      <c r="M2" s="4">
         <v>20.435199999999998</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
@@ -1642,37 +1666,43 @@
       <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="4">
         <v>56.470471000000003</v>
       </c>
-      <c r="G3" s="4">
+      <c r="I3" s="4">
         <v>-3.1227999999999998</v>
       </c>
-      <c r="H3" s="4">
+      <c r="J3" s="4">
         <v>26.4</v>
       </c>
-      <c r="I3" s="4">
+      <c r="K3" s="4">
         <v>17.075500000000002</v>
       </c>
-      <c r="J3" s="4">
+      <c r="L3" s="4">
         <v>8</v>
       </c>
-      <c r="K3" s="4">
+      <c r="M3" s="4">
         <v>24.342500000000001</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -1680,37 +1710,43 @@
       <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="4">
         <v>56.465794000000002</v>
       </c>
-      <c r="G4" s="4">
+      <c r="I4" s="4">
         <v>-3.12696</v>
       </c>
-      <c r="H4" s="4">
+      <c r="J4" s="4">
         <v>98.1</v>
       </c>
-      <c r="I4" s="4">
+      <c r="K4" s="4">
         <v>5.6565000000000003</v>
       </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
         <v>10.432399999999999</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
@@ -1718,37 +1754,43 @@
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="4">
         <v>56.468415</v>
       </c>
-      <c r="G5" s="4">
+      <c r="I5" s="4">
         <v>-3.1256499999999998</v>
       </c>
-      <c r="H5" s="4">
+      <c r="J5" s="4">
         <v>76.5</v>
       </c>
-      <c r="I5" s="4">
+      <c r="K5" s="4">
         <v>6.4452999999999996</v>
       </c>
-      <c r="J5" s="4">
+      <c r="L5" s="4">
         <v>2</v>
       </c>
-      <c r="K5" s="4">
+      <c r="M5" s="4">
         <v>9.4054000000000002</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -1756,35 +1798,41 @@
       <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="4">
         <v>56.470269999999999</v>
       </c>
-      <c r="G6" s="4">
+      <c r="I6" s="4">
         <v>-3.1406999999999998</v>
       </c>
-      <c r="H6" s="4">
+      <c r="J6" s="4">
         <v>76.2</v>
       </c>
-      <c r="I6" s="4">
+      <c r="K6" s="4">
         <v>16.232500000000002</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4">
         <v>21.435600000000001</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4">
         <v>2</v>
@@ -1792,73 +1840,85 @@
       <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="4">
+        <v>56.471969000000001</v>
+      </c>
+      <c r="I7" s="4">
+        <v>-3.11985</v>
+      </c>
+      <c r="J7" s="4">
+        <v>62.4</v>
+      </c>
+      <c r="K7" s="4">
+        <v>17.552600000000002</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
+        <v>22.467400000000001</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="4">
-        <v>56.471969000000001</v>
-      </c>
-      <c r="G7" s="4">
-        <v>-3.11985</v>
-      </c>
-      <c r="H7" s="4">
-        <v>62.4</v>
-      </c>
-      <c r="I7" s="4">
-        <v>17.552600000000002</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4">
-        <v>22.467400000000001</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="4">
         <v>56.468760000000003</v>
       </c>
-      <c r="G8" s="4">
+      <c r="I8" s="4">
         <v>-3.1153</v>
       </c>
-      <c r="H8" s="4">
+      <c r="J8" s="4">
         <v>56.4</v>
       </c>
-      <c r="I8" s="4">
+      <c r="K8" s="4">
         <v>4.5321999999999996</v>
       </c>
-      <c r="J8" s="4">
+      <c r="L8" s="4">
         <v>2</v>
       </c>
-      <c r="K8" s="4">
+      <c r="M8" s="4">
         <v>16.546600000000002</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
@@ -1866,37 +1926,43 @@
       <c r="C9" s="4">
         <v>2</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="D9" s="4">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="4">
         <v>56.467841999999997</v>
       </c>
-      <c r="G9" s="4">
+      <c r="I9" s="4">
         <v>-3.1088</v>
       </c>
-      <c r="H9" s="4">
+      <c r="J9" s="4">
         <v>68.900000000000006</v>
       </c>
-      <c r="I9" s="4">
+      <c r="K9" s="4">
         <v>6.3562000000000003</v>
       </c>
-      <c r="J9" s="4">
+      <c r="L9" s="4">
         <v>3</v>
       </c>
-      <c r="K9" s="4">
+      <c r="M9" s="4">
         <v>15.545299999999999</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -1904,37 +1970,43 @@
       <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="4">
         <v>56.469270999999999</v>
       </c>
-      <c r="G10" s="4">
+      <c r="I10" s="4">
         <v>-3.14317</v>
       </c>
-      <c r="H10" s="4">
+      <c r="J10" s="4">
         <v>85.6</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>14.5463</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>6</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>24.545300000000001</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
@@ -1942,67 +2014,79 @@
       <c r="C11" s="4">
         <v>2</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="4">
+        <v>56.472653000000001</v>
+      </c>
+      <c r="I11" s="4">
+        <v>-3.1432699999999998</v>
+      </c>
+      <c r="J11" s="4">
+        <v>23.6</v>
+      </c>
+      <c r="K11">
+        <v>20.435600000000001</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>25.5366</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" s="4">
-        <v>56.472653000000001</v>
-      </c>
-      <c r="G11" s="4">
-        <v>-3.1432699999999998</v>
-      </c>
-      <c r="H11" s="4">
-        <v>23.6</v>
-      </c>
-      <c r="I11">
-        <v>20.435600000000001</v>
-      </c>
-      <c r="J11">
-        <v>8</v>
-      </c>
-      <c r="K11">
-        <v>25.5366</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="4">
         <v>56.461801000000001</v>
       </c>
-      <c r="G12" s="4">
+      <c r="I12" s="4">
         <v>-3.1385399999999999</v>
       </c>
-      <c r="H12" s="4">
+      <c r="J12" s="4">
         <v>85.9</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>9.4344999999999999</v>
       </c>
-      <c r="L12" s="4" t="s">
-        <v>83</v>
+      <c r="N12" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2043,39 +2127,39 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2084,10 +2168,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" s="4">
         <v>56.46152</v>
@@ -2110,7 +2194,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
@@ -2119,10 +2203,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="4">
         <v>56.470471000000003</v>
@@ -2145,7 +2229,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -2154,10 +2238,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="4">
         <v>56.465794000000002</v>
@@ -2180,7 +2264,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
@@ -2189,10 +2273,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F5" s="4">
         <v>56.468415</v>
@@ -2215,7 +2299,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -2224,10 +2308,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" s="4">
         <v>56.470269999999999</v>
@@ -2248,7 +2332,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4">
         <v>2</v>
@@ -2257,10 +2341,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" s="4">
         <v>56.471969000000001</v>
@@ -2281,7 +2365,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -2290,10 +2374,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" s="4">
         <v>56.468760000000003</v>
@@ -2316,7 +2400,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
@@ -2325,10 +2409,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F9" s="4">
         <v>56.467841999999997</v>
@@ -2351,7 +2435,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -2360,10 +2444,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F10" s="4">
         <v>56.469270999999999</v>
@@ -2386,7 +2470,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
@@ -2395,10 +2479,10 @@
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11" s="4">
         <v>56.472653000000001</v>
@@ -2421,7 +2505,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
@@ -2430,10 +2514,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" s="4">
         <v>56.461801000000001</v>
@@ -2497,205 +2581,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829331A2-8F6C-4EC4-B723-84C59F96FDF0}">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H2" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H3" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H4" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{A99E7B79-269E-427E-A290-9658276FC0EE}">
-      <formula1>$H$2:$H$5</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C867D861-9536-4856-8988-38BB3B3563D5}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="ISO 3166-1 alpha-2" prompt="https://en.wikipedia.org/wiki/ISO_3166-1_alpha-2_x000a_" sqref="C1" xr:uid="{0D9EB899-F3F3-4ABD-A285-8DBAE030C105}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2115B6D0-8EC1-4029-B8F6-04E7D9736B3A}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="42.42578125" style="23" customWidth="1"/>
-    <col min="2" max="4" width="40.85546875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="23" customWidth="1"/>
-    <col min="8" max="8" width="25" style="23" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -2720,7 +2605,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -2729,7 +2614,7 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -2742,16 +2627,16 @@
         <v>9</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="L1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2763,7 +2648,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="L2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2775,7 +2660,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="L3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2787,17 +2672,17 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="L4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2 D2">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2822,107 +2707,118 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="9" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="H1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2937,60 +2833,271 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="H1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
   </sheetData>
   <dataValidations xWindow="96" yWindow="450" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:D1" xr:uid="{13E30841-E8AE-4AEA-9BB5-750247107F69}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:F1" xr:uid="{13E30841-E8AE-4AEA-9BB5-750247107F69}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829331A2-8F6C-4EC4-B723-84C59F96FDF0}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{A99E7B79-269E-427E-A290-9658276FC0EE}">
+      <formula1>$H$2:$H$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2115B6D0-8EC1-4029-B8F6-04E7D9736B3A}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.42578125" style="22" customWidth="1"/>
+    <col min="2" max="4" width="40.85546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="25" style="22" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="22" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C867D861-9536-4856-8988-38BB3B3563D5}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="ISO 3166-1 alpha-2" prompt="https://en.wikipedia.org/wiki/ISO_3166-1_alpha-2_x000a_" sqref="C1" xr:uid="{0D9EB899-F3F3-4ABD-A285-8DBAE030C105}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3013,30 +3120,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="D2" s="4">
         <v>30</v>
@@ -3050,13 +3157,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="4">
         <v>140</v>
@@ -3130,7 +3237,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -3139,7 +3246,7 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -3152,99 +3259,99 @@
         <v>9</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
         <v>81</v>
-      </c>
-      <c r="C5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>